<commit_message>
rajout de tests matt
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>numéro</t>
   </si>
@@ -341,6 +341,63 @@
   </si>
   <si>
     <t>testBaseCharFullLifeCours</t>
+  </si>
+  <si>
+    <t>Plateau</t>
+  </si>
+  <si>
+    <t>testDimensionsDebut</t>
+  </si>
+  <si>
+    <t>validé si le plateau est bien de la dimension entrée en paramètres au début de la partie</t>
+  </si>
+  <si>
+    <t>testDimensionsCours</t>
+  </si>
+  <si>
+    <t>validé si le plateau fait toujours la même dimension au cours de cette même partie</t>
+  </si>
+  <si>
+    <t>testObstacles</t>
+  </si>
+  <si>
+    <t>validé si le plateau contient bien le bon pourcentage d'obstacles entré en paramètre au début de la partie</t>
+  </si>
+  <si>
+    <t>testBasesDebut</t>
+  </si>
+  <si>
+    <t>testBasesCours</t>
+  </si>
+  <si>
+    <t>validé si les bases sont situées aux extrémités d'une diagonale au début de la partie</t>
+  </si>
+  <si>
+    <t>validé si les bases sont situées sur les même cases qu'au début de cette même partie</t>
+  </si>
+  <si>
+    <t>testSortieImpossibleDebut</t>
+  </si>
+  <si>
+    <t>validé si la sortie de plateau par chaque côté est impossible au début de la partie</t>
+  </si>
+  <si>
+    <t>testSortieImpossibleTireur</t>
+  </si>
+  <si>
+    <t>validé si un tireur ne peut pas sortir du plateau en cours de partie</t>
+  </si>
+  <si>
+    <t>testSortieImpossiblePiegeur</t>
+  </si>
+  <si>
+    <t>validé si un piégeur ne peut pas sortir du plateau en cours de partie</t>
+  </si>
+  <si>
+    <t>testSortieImpossibleChar</t>
+  </si>
+  <si>
+    <t>validé si un char ne peut pas sortir du plateau en cours de partie</t>
   </si>
 </sst>
 </file>
@@ -705,10 +762,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,6 +1262,83 @@
         <v>95</v>
       </c>
     </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Prog Matt""
This reverts commit 7da80da100cccacdc1a4ee5221c122a70a7199cb.
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Prog Matt"""
This reverts commit 3062c125ed005b3e10b6677666d9410a3d10a73e.
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Prog Matt""""
This reverts commit 9dd04675543e967fbc621c1315923d82e63d77c4.
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "Prog Matt"""""
This reverts commit 8a73aef580ece63a4f9a47124162e6c627f5801f.
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "Revert "Prog Matt""""""
This reverts commit db48384bfc4bc034a6058eaf85f1cd53ada60cc7.
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "Revert "Revert "Prog Matt"""""""
This reverts commit f9a2c41cc94aa58de94fd8409ec5693baa09013e.
</commit_message>
<xml_diff>
--- a/spec/tests/cahier de test by matt.xlsx
+++ b/spec/tests/cahier de test by matt.xlsx
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>